<commit_message>
added infra for healenium
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testdata1.xlsx
+++ b/src/test/resources/TestData/testdata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="687"/>
+    <workbookView windowWidth="19200" windowHeight="6800" tabRatio="687" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestDataMobile" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="130">
   <si>
     <t>DataID</t>
   </si>
@@ -163,13 +163,16 @@
     <t>MS003</t>
   </si>
   <si>
-    <t>b88be5542609</t>
-  </si>
-  <si>
-    <t>com.darwinuxmobile</t>
-  </si>
-  <si>
-    <t>com.darwinuxmobile.MainActivity</t>
+    <t>Galaxy A71</t>
+  </si>
+  <si>
+    <t>RZ8N21G4DTP</t>
+  </si>
+  <si>
+    <t>com.starbucks.in.beta</t>
+  </si>
+  <si>
+    <t>com.tsb.app.home.presentation.view.activity.HomeActivity</t>
   </si>
   <si>
     <t>MS005</t>
@@ -1492,8 +1495,8 @@
   <sheetPr/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83636363636364" defaultRowHeight="14.5" outlineLevelCol="4"/>
@@ -1669,7 +1672,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16363636363636" defaultRowHeight="14.5"/>
@@ -1686,7 +1689,7 @@
     <col min="10" max="10" width="21.6636363636364" style="13" customWidth="1"/>
     <col min="11" max="11" width="24.5090909090909" style="13" customWidth="1"/>
     <col min="12" max="12" width="93.3363636363636" style="13" customWidth="1"/>
-    <col min="13" max="13" width="19.0090909090909" style="13" customWidth="1"/>
+    <col min="13" max="13" width="19" style="13" customWidth="1"/>
     <col min="14" max="14" width="28.9090909090909" style="13" customWidth="1"/>
     <col min="15" max="15" width="18.5090909090909" style="13" customWidth="1"/>
     <col min="16" max="16" width="13.6636363636364" style="13" customWidth="1"/>
@@ -1834,41 +1837,39 @@
       <c r="B5" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17">
+        <v>13</v>
+      </c>
       <c r="D5" s="17"/>
       <c r="E5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="17" t="b">
-        <v>0</v>
-      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
       <c r="H5" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17">
-        <v>120</v>
-      </c>
+      <c r="I5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="17"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N5" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" s="17">
         <v>14.7</v>
@@ -1879,10 +1880,10 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
@@ -1890,7 +1891,7 @@
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
       <c r="O6" s="23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P6" s="18" t="b">
         <v>1</v>
@@ -1901,7 +1902,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="17">
         <v>14.6</v>
@@ -1920,7 +1921,7 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P7" s="18" t="b">
         <v>1</v>
@@ -1928,16 +1929,16 @@
     </row>
     <row r="8" s="13" customFormat="1" spans="1:14">
       <c r="A8" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="17">
         <v>14.7</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>36</v>
@@ -1949,15 +1950,15 @@
         <v>38</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J8" s="17"/>
       <c r="K8" s="21"/>
       <c r="L8" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
@@ -2082,8 +2083,8 @@
   <sheetPr/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
@@ -2098,35 +2099,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:3">
       <c r="A2" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:3">
       <c r="A3" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="11"/>
     </row>
     <row r="4" customFormat="1" spans="1:3">
       <c r="A4" s="12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -2193,49 +2194,49 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" ht="87" spans="1:4">
       <c r="A3" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B4" s="12">
         <v>1</v>
@@ -2244,12 +2245,12 @@
         <v>11</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B5" s="12">
         <v>2</v>
@@ -2258,12 +2259,12 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="12">
         <v>3</v>
@@ -2272,12 +2273,12 @@
         <v>33</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B7" s="12">
         <v>4</v>
@@ -2286,12 +2287,12 @@
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B8" s="12">
         <v>5</v>
@@ -2300,12 +2301,12 @@
         <v>55</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B9" s="12">
         <v>6</v>
@@ -2314,12 +2315,12 @@
         <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="12">
         <v>7</v>
@@ -2328,12 +2329,12 @@
         <v>77</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B11" s="12">
         <v>8</v>
@@ -2342,12 +2343,12 @@
         <v>88</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" s="12">
         <v>9</v>
@@ -2356,12 +2357,12 @@
         <v>99</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B13" s="12">
         <v>10</v>
@@ -2370,12 +2371,12 @@
         <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" s="12">
         <v>11</v>
@@ -2384,12 +2385,12 @@
         <v>111</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B15" s="12">
         <v>12</v>
@@ -2398,12 +2399,12 @@
         <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B16" s="12">
         <v>13</v>
@@ -2412,12 +2413,12 @@
         <v>113</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="12">
         <v>14</v>
@@ -2426,12 +2427,12 @@
         <v>114</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" s="12">
         <v>15</v>
@@ -2440,12 +2441,12 @@
         <v>115</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B19" s="12">
         <v>16</v>
@@ -2454,12 +2455,12 @@
         <v>116</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" s="12">
         <v>17</v>
@@ -2468,12 +2469,12 @@
         <v>117</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B21" s="12">
         <v>18</v>
@@ -2482,12 +2483,12 @@
         <v>118</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B22" s="12">
         <v>19</v>
@@ -2496,12 +2497,12 @@
         <v>119</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" s="12">
         <v>20</v>
@@ -2510,12 +2511,12 @@
         <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" s="12">
         <v>21</v>
@@ -2524,12 +2525,12 @@
         <v>121</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B25" s="12">
         <v>22</v>
@@ -2538,12 +2539,12 @@
         <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26" s="12">
         <v>23</v>
@@ -2552,12 +2553,12 @@
         <v>123</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B27" s="12">
         <v>24</v>
@@ -2566,12 +2567,12 @@
         <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" s="12">
         <v>25</v>
@@ -2580,12 +2581,12 @@
         <v>125</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B29" s="12">
         <v>26</v>
@@ -2594,12 +2595,12 @@
         <v>126</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B30" s="12">
         <v>27</v>
@@ -2608,12 +2609,12 @@
         <v>127</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B31" s="12">
         <v>28</v>
@@ -2622,12 +2623,12 @@
         <v>128</v>
       </c>
       <c r="D31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B32" s="12">
         <v>29</v>
@@ -2636,12 +2637,12 @@
         <v>129</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B33" s="12">
         <v>30</v>
@@ -2650,12 +2651,12 @@
         <v>330</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B34" s="12">
         <v>31</v>
@@ -2664,12 +2665,12 @@
         <v>341</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35" s="12">
         <v>32</v>
@@ -2678,12 +2679,12 @@
         <v>352</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B36" s="12">
         <v>33</v>
@@ -2692,12 +2693,12 @@
         <v>363</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B37" s="12">
         <v>34</v>
@@ -2706,12 +2707,12 @@
         <v>374</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B38" s="12">
         <v>35</v>
@@ -2720,12 +2721,12 @@
         <v>385</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B39" s="12">
         <v>36</v>
@@ -2734,12 +2735,12 @@
         <v>396</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B40" s="12">
         <v>37</v>
@@ -2748,12 +2749,12 @@
         <v>407</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B41" s="12">
         <v>38</v>
@@ -2762,12 +2763,12 @@
         <v>418</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B42" s="12">
         <v>39</v>
@@ -2776,12 +2777,12 @@
         <v>429</v>
       </c>
       <c r="D42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B43" s="12">
         <v>40</v>
@@ -2790,12 +2791,12 @@
         <v>440</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B44" s="12">
         <v>41</v>
@@ -2804,12 +2805,12 @@
         <v>451</v>
       </c>
       <c r="D44" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B45" s="12">
         <v>42</v>
@@ -2818,12 +2819,12 @@
         <v>462</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B46" s="12">
         <v>43</v>
@@ -2832,12 +2833,12 @@
         <v>473</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B47" s="12">
         <v>44</v>
@@ -2846,12 +2847,12 @@
         <v>484</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B48" s="12">
         <v>45</v>
@@ -2860,12 +2861,12 @@
         <v>495</v>
       </c>
       <c r="D48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B49" s="12">
         <v>46</v>
@@ -2874,12 +2875,12 @@
         <v>506</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B50" s="12">
         <v>47</v>
@@ -2888,12 +2889,12 @@
         <v>517</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B51" s="12">
         <v>48</v>
@@ -2902,7 +2903,7 @@
         <v>528</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2942,64 +2943,64 @@
   <sheetData>
     <row r="1" ht="15" spans="1:17">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2">
         <v>40000</v>
@@ -3023,19 +3024,19 @@
         <v>500000</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3072,51 +3073,51 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3">
         <v>100010</v>
@@ -3125,40 +3126,40 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J2" s="3">
         <v>200</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M2" s="3">
         <v>100010</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B3" s="3">
         <v>100011</v>
@@ -3167,22 +3168,22 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J3" s="3">
         <v>200</v>
@@ -3196,31 +3197,31 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B4" s="3">
         <v>100012</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E4" s="3">
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J4" s="3">
         <v>500</v>
@@ -3234,7 +3235,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B5" s="3">
         <v>100013</v>
@@ -3243,22 +3244,22 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J5" s="3">
         <v>200</v>
@@ -3272,7 +3273,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B6" s="3">
         <v>100014</v>
@@ -3281,22 +3282,22 @@
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J6" s="3">
         <v>500</v>
@@ -3310,7 +3311,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B7" s="3">
         <v>100015</v>
@@ -3319,22 +3320,22 @@
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J7" s="3">
         <v>200</v>

</xml_diff>